<commit_message>
Trying to solve commit problems by cloning the remote repo and manually consolidating with local repo
</commit_message>
<xml_diff>
--- a/Writing/Tables/simulationTable.xlsx
+++ b/Writing/Tables/simulationTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Dropbox\CJM\Masterproject\Writing\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\projects\2014toogoodtobefalse\Writing\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -492,188 +492,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">

</xml_diff>